<commit_message>
add Test Case Explanation.txt update test data
</commit_message>
<xml_diff>
--- a/factorialCalculator/src/test/java/testData/testData.xlsx
+++ b/factorialCalculator/src/test/java/testData/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23451" windowHeight="11974"/>
+    <workbookView windowWidth="12780" windowHeight="11382"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,15 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t xml:space="preserve">input </t>
   </si>
   <si>
     <t>expectedResult</t>
-  </si>
-  <si>
-    <t>actualResult</t>
   </si>
   <si>
     <t>The factorial of 0 is: 1</t>
@@ -40,7 +37,7 @@
     <t>The factorial of 190 is: Infinity</t>
   </si>
   <si>
-    <t>NA</t>
+    <t>no response currently</t>
   </si>
 </sst>
 </file>
@@ -985,27 +982,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.61261261261261" defaultRowHeight="14.55" outlineLevelRow="6" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.61261261261261" defaultRowHeight="14.55" outlineLevelRow="7" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="8.61261261261261" style="1"/>
     <col min="2" max="2" width="32.036036036036" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1013,7 +1007,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1021,7 +1015,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1029,7 +1023,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1037,7 +1031,7 @@
         <v>189</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1045,7 +1039,7 @@
         <v>190</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1053,7 +1047,15 @@
         <v>-2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>